<commit_message>
Preparing to change extend_to_exergy()
</commit_message>
<xml_diff>
--- a/inst/extdata/Testing_irreversibility/Testing_irreversibility.xlsx
+++ b/inst/extdata/Testing_irreversibility/Testing_irreversibility.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/Recca/inst/extdata/Testing_irreversibility/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73C2362-6227-C14F-ADD8-8CF76F59E9C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDE6491-3657-A442-BE81-635EFB5B3873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="50020" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="50020" windowHeight="28300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="10" r:id="rId1"/>
@@ -1169,7 +1169,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37160BD0-5B0C-8D4D-B8AE-80F4F54225B9}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
@@ -6624,8 +6624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9273644-B629-5F45-9A68-323450968119}">
   <dimension ref="A1:IG87"/>
   <sheetViews>
-    <sheetView zoomScale="88" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="FB20" zoomScale="88" workbookViewId="0">
+      <selection activeCell="GI42" sqref="GI42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>